<commit_message>
[FIX/CHANGE] -Réparation de BUG concernant la vue "projet.html" et "veille.html" -Modification de la vue "veille.html"
</commit_message>
<xml_diff>
--- a/assets/Tableau de synthèse - Epreuve E4 Khatir SEDJAI.xlsx
+++ b/assets/Tableau de synthèse - Epreuve E4 Khatir SEDJAI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atixitfr-my.sharepoint.com/personal/ksedjai_atixit_fr/Documents/Documents/Portfolio/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{B71F6BA3-1B59-4660-BA92-ADE765BF1A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDC4EA35-E9BE-4A12-8B81-38525B269D3D}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="13_ncr:1_{B71F6BA3-1B59-4660-BA92-ADE765BF1A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54BCE70F-68FC-4EDA-8CC1-E85BE9A96BD6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>NOM et prénom : SEDJAI Khatir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N° candidat : </t>
   </si>
   <si>
     <t>Centre de formation : Lycée Robert Schuman</t>
@@ -132,25 +129,6 @@
 </t>
   </si>
   <si>
-    <t>Projet PHP: Gestion bibliothèque</t>
-  </si>
-  <si>
-    <t>03/2023 au 05/2023</t>
-  </si>
-  <si>
-    <t>Projet JAVAFX: ToDoList</t>
-  </si>
-  <si>
-    <t>04/23 au 12/05/2023</t>
-  </si>
-  <si>
-    <t>Projet E5 PHP: Développement d'une plateforme de gestion d'un reseau universitaire entre etudiant et entreprise. Ainsi que la _x000D_gesttion d'évenement 
-et de rendez-vous</t>
-  </si>
-  <si>
-    <t>En cours</t>
-  </si>
-  <si>
     <t>Veille Technologique</t>
   </si>
   <si>
@@ -178,16 +156,76 @@
     <t>Adresse URL du portfolio : https://khatirsedjai.github.io/Portfolio/</t>
   </si>
   <si>
-    <t>Création et gestion d'application via Power Apps</t>
-  </si>
-  <si>
-    <t>Création, maintenance et déploiement de Sites web (https://21daychallenge.fr/ et https://onetime.atixit.net/)</t>
-  </si>
-  <si>
-    <t>Contribution et optimisation aux applications pré-existantes</t>
-  </si>
-  <si>
     <t>Contribution et optimisation des sites web pré-existants</t>
+  </si>
+  <si>
+    <t>SIO 1 SEMESTRE 1 - Création d'un pendu en JAVA</t>
+  </si>
+  <si>
+    <t>SIO 1 SEMESTRE 1 - Mise en place et utilisation du CMS WordPress</t>
+  </si>
+  <si>
+    <t>SIO 1 SEMESTRE 1 - Introduction et déploiement du framework Symfony</t>
+  </si>
+  <si>
+    <t>SIO 1 SEMESTRE 2 - Création et déploiement d'un Portfolio</t>
+  </si>
+  <si>
+    <t>SIO 1 SEMESTRE 2 - Création d'un site dédié à la gestion d'une bibliothèque en PHP</t>
+  </si>
+  <si>
+    <t>SIO 1 SEMESTRE 2 - Conception d'une application lourde avec gestion des opérations CRUD pour les utilisateurs réalisée en JAVA et JAVAFX</t>
+  </si>
+  <si>
+    <t>SIO 1 SEMESTRE 2 - Conception d'une application de gestion de tâches (To Do List) en environnement client lourd réalisée en JAVA et JAVA FX</t>
+  </si>
+  <si>
+    <t>SIO 2 SEMESTRE 2 - Projet Épreuve E5 - Conception et mise en ligne d'un site web dédié à la gestion des relations entre les établissements universitaires/lycées et les entreprises</t>
+  </si>
+  <si>
+    <t>SIO 2 SEMESTRE 2 - Projet Épreuve E5 - Conception d'une application lourde en JAVAFX pour la gestion de stock d'une école</t>
+  </si>
+  <si>
+    <t>Création, maintenance et déploiement de Sites web en php avec le framework Laravel vie Plesk (https://21daychallenge.fr/ et https://onetime.atixit.net/)</t>
+  </si>
+  <si>
+    <t>Contribution et optimisation des applications pré-existantes</t>
+  </si>
+  <si>
+    <t>Création, gestion et déploiement de version d'application via Power Apps</t>
+  </si>
+  <si>
+    <t>21/10/2022 au 07/11/2022</t>
+  </si>
+  <si>
+    <t>21/11/2022 au 25/05/2022</t>
+  </si>
+  <si>
+    <t>13/12/2022 au 20/12/2022</t>
+  </si>
+  <si>
+    <t>12/05/2023 au 12/06/2023</t>
+  </si>
+  <si>
+    <t>09/01/2023 au 11/07/2024</t>
+  </si>
+  <si>
+    <t>01/09/2022 au 11/07/2024</t>
+  </si>
+  <si>
+    <t>16/02/2023 au 13/03/2023</t>
+  </si>
+  <si>
+    <t>19/04/2023 au 05/05/2023</t>
+  </si>
+  <si>
+    <t>01/09/2023 au 15/12/2023</t>
+  </si>
+  <si>
+    <t>15/12/2023 au 20/03/2024</t>
+  </si>
+  <si>
+    <t>N° candidat : 02047333096</t>
   </si>
 </sst>
 </file>
@@ -255,7 +293,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="16"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -264,13 +309,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -282,13 +321,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -725,9 +764,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -746,25 +782,28 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -847,6 +886,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1141,14 +1184,14 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" style="1" customWidth="1"/>
     <col min="3" max="8" width="18.6640625" style="1" customWidth="1"/>
     <col min="9" max="43" width="11.44140625" customWidth="1"/>
     <col min="44" max="16384" width="10.88671875" style="1"/>
@@ -1189,7 +1232,7 @@
       <c r="D3" s="30"/>
       <c r="E3" s="31"/>
       <c r="F3" s="35" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="G3" s="30"/>
       <c r="H3" s="36"/>
@@ -1199,25 +1242,25 @@
     </row>
     <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
       <c r="E4" s="34"/>
       <c r="F4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="18" t="s">
         <v>7</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
@@ -1229,50 +1272,50 @@
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="38"/>
       <c r="B7" s="46"/>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="E7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="F7" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="G7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="H7" s="22" t="s">
         <v>21</v>
-      </c>
-      <c r="H7" s="26" t="s">
-        <v>22</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1312,7 +1355,7 @@
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="40"/>
       <c r="C8" s="40"/>
@@ -1359,17 +1402,17 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
+        <v>33</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="25"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1407,18 +1450,18 @@
       <c r="AQ9"/>
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
-        <v>26</v>
+      <c r="A10" s="20" t="s">
+        <v>34</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
+        <v>46</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1457,17 +1500,17 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22"/>
+        <v>47</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="25"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1506,17 +1549,17 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="22"/>
+        <v>36</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1554,14 +1597,18 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16"/>
+      <c r="A13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="24"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="15"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1599,14 +1646,18 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="16"/>
+      <c r="A14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="24"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="15"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1644,14 +1695,18 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="16"/>
+      <c r="A15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="24"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="15"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1689,14 +1744,17 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="16"/>
+      <c r="A16" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="24"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1734,14 +1792,18 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="16"/>
+      <c r="A17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="15"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1779,14 +1841,18 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="16"/>
+      <c r="A18" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="15"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1825,7 +1891,7 @@
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B19" s="43"/>
       <c r="C19" s="43"/>
@@ -1872,17 +1938,17 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="16"/>
+        <v>26</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="15"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -1921,17 +1987,17 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="16"/>
+        <v>26</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="15"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -1971,12 +2037,12 @@
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="8"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="16"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="15"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -2016,12 +2082,12 @@
     <row r="23" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="8"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="16"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="15"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2061,12 +2127,12 @@
     <row r="24" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="16"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="15"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2106,12 +2172,12 @@
     <row r="25" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="16"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="15"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2151,12 +2217,12 @@
     <row r="26" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="8"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="16"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="15"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2195,7 +2261,7 @@
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A27" s="42" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B27" s="43"/>
       <c r="C27" s="43"/>
@@ -2242,17 +2308,17 @@
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
+        <v>29</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2291,17 +2357,17 @@
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="16"/>
+        <v>29</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="15"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2340,17 +2406,17 @@
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="16"/>
+        <v>29</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="15"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2389,17 +2455,17 @@
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="27"/>
+        <v>29</v>
+      </c>
+      <c r="C31" s="24"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="23"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2438,17 +2504,17 @@
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="16"/>
+        <v>29</v>
+      </c>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="15"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2488,12 +2554,12 @@
     <row r="33" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="8"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="16"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="15"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2533,12 +2599,12 @@
     <row r="34" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="18"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="17"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>

</xml_diff>